<commit_message>
v0.23.0 - Replace PoD-qx with LT-qx and re-generate the GBD life tables. Also, tune down the Kannisto modelling to extend mortality w/o altering the existing life-table results since these match already pretty well the HMD.
</commit_message>
<xml_diff>
--- a/data-raw/IHME_GBD2021_Data/GBD2021_Download_Selection_Settings.xlsx
+++ b/data-raw/IHME_GBD2021_Data/GBD2021_Download_Selection_Settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dump_\Documents\R-REPOS\lemur\data-raw\IHME_GBD2021_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dump_\WORKSPACE\CODE\R-REPOS\lemur\data-raw\IHME_GBD2021_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF1B0BD-2D32-46C2-B614-D8CEB0F87690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93607688-D0E2-4ED9-9BD2-5B5CE5DAD260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C6CB6211-8AB1-420C-A7DD-D1AA880F132F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t xml:space="preserve"> GBD Results tool:</t>
   </si>
@@ -137,13 +137,7 @@
     <t>Female</t>
   </si>
   <si>
-    <t>Probability of death, by cause</t>
-  </si>
-  <si>
     <t>Probability of death</t>
-  </si>
-  <si>
-    <t>All causes</t>
   </si>
   <si>
     <t>Male, Female, Both</t>
@@ -191,9 +185,6 @@
     <t>8e2070ba8a0967120684cd25bfeefde9</t>
   </si>
   <si>
-    <t>ce35093f4329036573f7b552d610ca4f</t>
-  </si>
-  <si>
     <t>Results Token ID</t>
   </si>
   <si>
@@ -204,12 +195,17 @@
   </si>
   <si>
     <t>114e4fdd5c8d25af41d7c72a6373bf87</t>
+  </si>
+  <si>
+    <t>All-cause mortality</t>
+  </si>
+  <si>
+    <t>LT</t>
   </si>
   <si>
     <t>"Select all countries and teritories"
 Global
 African Union
-Central Africa
 Association of Southeast Asian Nations
 Commonwealth
 European Union
@@ -220,16 +216,20 @@
 G20
 Gulf Cooperation Council
 League of Arab States
+Nordic Region
 OECD Countries
 Organization of Islamic Cooperation
 Sahel Region</t>
+  </si>
+  <si>
+    <t>6cbbe744b9a9b097843f2119811a8f8d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +274,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF454545"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -329,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -368,6 +375,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,6 +396,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>227457</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>3157577</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{691BBE77-8EDE-FFD7-9B73-31EA998B1684}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21078265" y="3104029"/>
+          <a:ext cx="3858163" cy="6306430"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>89648</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85127</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2297206</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90CBB28A-B1E9-3192-6433-4772E06F3713}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11317942" y="11728039"/>
+          <a:ext cx="2207558" cy="4296372"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -689,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532DC562-4BE8-41D8-BFCB-8343057AE96B}">
   <dimension ref="C2:I20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,16 +833,16 @@
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="3:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="9"/>
       <c r="D10" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>17</v>
@@ -774,7 +875,7 @@
         <v>Cause of death or Injury</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>15</v>
@@ -798,7 +899,7 @@
         <v>Deaths</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>25</v>
@@ -822,7 +923,7 @@
         <v>Number</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>21</v>
@@ -836,16 +937,16 @@
         <v>9</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>26</v>
@@ -859,20 +960,13 @@
         <v>10</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="5" t="str">
-        <f>F15</f>
+        <v>47</v>
+      </c>
+      <c r="E15" s="5" t="str">
+        <f t="shared" ref="E15:F15" si="0">D15</f>
         <v>"Select all countries and teritories"
 Global
 African Union
-Central Africa
 Association of Southeast Asian Nations
 Commonwealth
 European Union
@@ -883,16 +977,16 @@
 G20
 Gulf Cooperation Council
 League of Arab States
+Nordic Region
 OECD Countries
 Organization of Islamic Cooperation
 Sahel Region</v>
       </c>
-      <c r="H15" s="5" t="str">
-        <f>G15</f>
+      <c r="F15" s="5" t="str">
+        <f t="shared" si="0"/>
         <v>"Select all countries and teritories"
 Global
 African Union
-Central Africa
 Association of Southeast Asian Nations
 Commonwealth
 European Union
@@ -903,16 +997,16 @@
 G20
 Gulf Cooperation Council
 League of Arab States
+Nordic Region
 OECD Countries
 Organization of Islamic Cooperation
 Sahel Region</v>
       </c>
-      <c r="I15" s="5" t="str">
-        <f>H15</f>
+      <c r="G15" s="5" t="str">
+        <f>F15</f>
         <v>"Select all countries and teritories"
 Global
 African Union
-Central Africa
 Association of Southeast Asian Nations
 Commonwealth
 European Union
@@ -923,26 +1017,67 @@
 G20
 Gulf Cooperation Council
 League of Arab States
+Nordic Region
 OECD Countries
 Organization of Islamic Cooperation
 Sahel Region</v>
       </c>
+      <c r="H15" s="5" t="str">
+        <f>G15</f>
+        <v>"Select all countries and teritories"
+Global
+African Union
+Association of Southeast Asian Nations
+Commonwealth
+European Union
+Africa
+America
+Asia
+Europe
+G20
+Gulf Cooperation Council
+League of Arab States
+Nordic Region
+OECD Countries
+Organization of Islamic Cooperation
+Sahel Region</v>
+      </c>
+      <c r="I15" s="5" t="str">
+        <f>H15</f>
+        <v>"Select all countries and teritories"
+Global
+African Union
+Association of Southeast Asian Nations
+Commonwealth
+European Union
+Africa
+America
+Asia
+Europe
+G20
+Gulf Cooperation Council
+League of Arab States
+Nordic Region
+OECD Countries
+Organization of Islamic Cooperation
+Sahel Region</v>
+      </c>
     </row>
     <row r="16" spans="3:9" ht="345" x14ac:dyDescent="0.25">
       <c r="C16" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>27</v>
@@ -966,7 +1101,7 @@
         <v>Male, Female</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>28</v>
@@ -1006,22 +1141,23 @@
     </row>
     <row r="20" spans="3:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C20" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" t="s">
-        <v>43</v>
+      <c r="G20" s="18" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>